<commit_message>
Load brand from database dynamic from production controller. User production repository extension to get all production brand
</commit_message>
<xml_diff>
--- a/Mybrus/App_Data/Coluc.xlsx
+++ b/Mybrus/App_Data/Coluc.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>Task Name</t>
   </si>
@@ -263,10 +263,16 @@
     <t>Redesign</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Extended</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Sample data</t>
   </si>
 </sst>
 </file>
@@ -613,44 +619,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -664,9 +682,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,15 +708,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1018,7 +1024,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,34 +1039,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="27"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1073,25 +1079,25 @@
       <c r="K2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="42" t="s">
-        <v>57</v>
+      <c r="L2" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="7">
         <v>42093</v>
       </c>
@@ -1104,25 +1110,25 @@
       <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="23" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="7">
         <v>42098</v>
       </c>
@@ -1135,23 +1141,23 @@
       <c r="K4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="L4" s="16" t="s">
         <v>55</v>
       </c>
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="7">
         <v>42108</v>
       </c>
@@ -1162,23 +1168,23 @@
         <v>42119</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="7">
         <v>42119</v>
       </c>
@@ -1188,22 +1194,24 @@
       <c r="J6" s="7">
         <v>42125</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="L6" s="13"/>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="23" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="7">
         <v>42125</v>
       </c>
@@ -1213,22 +1221,24 @@
       <c r="J7" s="7">
         <v>42135</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="7">
         <v>42135</v>
       </c>
@@ -1238,22 +1248,24 @@
       <c r="J8" s="7">
         <v>42140</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="L8" s="13"/>
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="7">
         <v>42142</v>
       </c>
@@ -1263,22 +1275,26 @@
       <c r="J9" s="7">
         <v>42149</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="7">
         <v>42150</v>
       </c>
@@ -1293,17 +1309,17 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="7">
         <v>42159</v>
       </c>
@@ -1313,22 +1329,24 @@
       <c r="J11" s="7">
         <v>42175</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="L11" s="13"/>
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="7">
         <v>42177</v>
       </c>
@@ -1343,17 +1361,17 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="7">
         <v>42186</v>
       </c>
@@ -1368,17 +1386,17 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="7">
         <v>42192</v>
       </c>
@@ -1388,22 +1406,24 @@
       <c r="J14" s="7">
         <v>42200</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="L14" s="13"/>
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="7">
         <v>42201</v>
       </c>
@@ -1418,45 +1438,45 @@
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -1465,13 +1485,13 @@
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
@@ -1480,13 +1500,13 @@
       <c r="M19" s="10"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
@@ -1495,13 +1515,13 @@
       <c r="M20" s="10"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
@@ -1510,13 +1530,13 @@
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -1525,13 +1545,13 @@
       <c r="M22" s="10"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -1540,13 +1560,13 @@
       <c r="M23" s="10"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
@@ -1555,13 +1575,13 @@
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
@@ -1570,13 +1590,13 @@
       <c r="M25" s="10"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -1585,13 +1605,13 @@
       <c r="M26" s="10"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -1600,13 +1620,13 @@
       <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
@@ -1615,13 +1635,13 @@
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
@@ -1630,13 +1650,13 @@
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
@@ -1646,6 +1666,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A16:M17"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D22:G22"/>
     <mergeCell ref="D29:G29"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="D30:G30"/>
@@ -1662,46 +1722,6 @@
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="D21:G21"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A16:M17"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M3" location="Sheet2!A1" display="Need confirm"/>
@@ -1728,201 +1748,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="28" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="38"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E2:G2"/>
@@ -1939,8 +1961,6 @@
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:J1" location="Sheet1!A1" display="Application Requests"/>

</xml_diff>